<commit_message>
In Klassen.xls Funktion printFleet hinzugefügt - Dino
</commit_message>
<xml_diff>
--- a/Product Description/Klassen.xlsx
+++ b/Product Description/Klassen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\IdeaProjects\TM22_SoftwareEngineering_Gruppe2\Product Description\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DinoG\OneDrive\Desktop\Technisches Management 3. Semester\Software Engineering ILV\Git\Product Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2644037C-43C6-496D-9896-DB1522D79A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B71460-5C3E-431E-B451-4D6174904069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{EAE77123-B87F-48FC-8583-1A6EE0A6B883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EAE77123-B87F-48FC-8583-1A6EE0A6B883}"/>
   </bookViews>
   <sheets>
     <sheet name="Klassen" sheetId="1" r:id="rId1"/>
@@ -39,38 +39,47 @@
     <author>tc={94C0B99F-C29B-43A8-935C-3212A1A77F9C}</author>
     <author>tc={FCDDE2B2-D921-4040-B134-94E9E6B087D0}</author>
     <author>tc={9287C3D1-697B-408A-BE6F-8850285BA640}</author>
+    <author>tc={8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}</author>
     <author>tc={0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}</author>
   </authors>
   <commentList>
     <comment ref="N10" authorId="0" shapeId="0" xr:uid="{94C0B99F-C29B-43A8-935C-3212A1A77F9C}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     creates ships randomly &amp; then sets it onto the field</t>
       </text>
     </comment>
     <comment ref="D11" authorId="1" shapeId="0" xr:uid="{FCDDE2B2-D921-4040-B134-94E9E6B087D0}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     Hier muss überprüft werden ob ship mit flotte kompatibel ist (ob nicht andere schiffe im Weg stehen ^^)</t>
       </text>
     </comment>
     <comment ref="N11" authorId="2" shapeId="0" xr:uid="{9287C3D1-697B-408A-BE6F-8850285BA640}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     sets all ships belonging to this fleet onto the field of the owner</t>
       </text>
     </comment>
-    <comment ref="D28" authorId="3" shapeId="0" xr:uid="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
+    <comment ref="N12" authorId="3" shapeId="0" xr:uid="{8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Bitte Funktion implementieren, damit wir die Fleet ausgeben können</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="4" shapeId="0" xr:uid="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     prints how many ships are sunk and how many are hit</t>
       </text>
     </comment>
@@ -79,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -262,6 +271,9 @@
   </si>
   <si>
     <t>createPlayer(name)</t>
+  </si>
+  <si>
+    <t>printFleet()</t>
   </si>
 </sst>
 </file>
@@ -302,7 +314,7 @@
     <font>
       <sz val="9"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
+      <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -563,18 +575,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,9 +590,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -609,12 +621,13 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Dino Ganic" id="{3BCCA9EA-61F7-4AAE-BD31-9F6FE5D618B8}" userId="4ed6363e1e8f2d27" providerId="Windows Live"/>
   <person displayName="adri würfl" id="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" userId="c6b28034b5dd424b" providerId="Windows Live"/>
 </personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -919,6 +932,9 @@
   <threadedComment ref="N11" dT="2021-09-25T13:55:58.73" personId="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" id="{9287C3D1-697B-408A-BE6F-8850285BA640}">
     <text>sets all ships belonging to this fleet onto the field of the owner</text>
   </threadedComment>
+  <threadedComment ref="N12" dT="2021-09-25T15:35:38.57" personId="{3BCCA9EA-61F7-4AAE-BD31-9F6FE5D618B8}" id="{8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}">
+    <text>Bitte Funktion implementieren, damit wir die Fleet ausgeben können</text>
+  </threadedComment>
   <threadedComment ref="D28" dT="2021-09-25T10:33:50.75" personId="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" id="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
     <text>prints how many ships are sunk and how many are hit</text>
   </threadedComment>
@@ -930,27 +946,27 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="1.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.77734375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C1" s="10"/>
       <c r="D1" s="11" t="s">
         <v>0</v>
@@ -982,31 +998,31 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="H3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
-      <c r="M3" s="22" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="20"/>
+      <c r="M3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="20"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
@@ -1041,7 +1057,7 @@
       </c>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -1072,7 +1088,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
@@ -1103,7 +1119,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
@@ -1118,7 +1134,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
@@ -1133,198 +1149,200 @@
       <c r="O8" s="4"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
       <c r="H9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="22"/>
       <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="26"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="O9" s="21"/>
+      <c r="P9" s="22"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
       <c r="H10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
       <c r="M10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="O10" s="23"/>
+      <c r="P10" s="24"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
       <c r="M11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="O11" s="23"/>
+      <c r="P11" s="24"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
       <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
       <c r="M12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="21"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N12" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="O12" s="23"/>
+      <c r="P12" s="24"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
       <c r="H13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
       <c r="M13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="24"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
       <c r="H14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="21"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
       <c r="M14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
-    </row>
-    <row r="15" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="24"/>
+    </row>
+    <row r="15" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="26"/>
       <c r="M15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="19"/>
-    </row>
-    <row r="17" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="18" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="26"/>
+    </row>
+    <row r="17" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="20"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="22" t="s">
+      <c r="M18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="24"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="20"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>1</v>
       </c>
@@ -1359,7 +1377,7 @@
       </c>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="C20" s="3" t="s">
         <v>4</v>
@@ -1394,7 +1412,7 @@
       </c>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="C21" s="3" t="s">
         <v>4</v>
@@ -1427,7 +1445,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
@@ -1442,7 +1460,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
@@ -1457,182 +1475,182 @@
       <c r="O23" s="4"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
       <c r="H24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
       <c r="M24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="26"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
       <c r="H25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
       <c r="M25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="21"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="24"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="C26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="24"/>
       <c r="H26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="24"/>
       <c r="M26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="21"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="24"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="C27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
       <c r="H27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="21"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="24"/>
       <c r="M27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="21"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="24"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="C28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="21"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
       <c r="M28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="21"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="24"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="C29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="H29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24"/>
       <c r="M29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="21"/>
-    </row>
-    <row r="30" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="24"/>
+    </row>
+    <row r="30" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="C30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="26"/>
       <c r="H30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="26"/>
       <c r="M30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="19"/>
-    </row>
-    <row r="32" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="33" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="26"/>
+    </row>
+    <row r="32" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="24"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>1</v>
       </c>
@@ -1647,7 +1665,7 @@
       </c>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="C35" s="3" t="s">
         <v>4</v>
@@ -1660,7 +1678,7 @@
       </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="C36" s="3" t="s">
         <v>4</v>
@@ -1673,149 +1691,108 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="26"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E39" s="21"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="C40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E40" s="23"/>
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="C41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="C42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E42" s="23"/>
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="C43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E43" s="23"/>
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="C44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="E44" s="23"/>
+      <c r="F44" s="24"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="15"/>
       <c r="C45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E45" s="23"/>
+      <c r="F45" s="24"/>
+    </row>
+    <row r="46" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
     <mergeCell ref="N30:P30"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="N10:P10"/>
@@ -1832,6 +1809,47 @@
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
In Klassen.xls Klasse Test und 2 Funktionen hinzugefügt - Dino
</commit_message>
<xml_diff>
--- a/Product Description/Klassen.xlsx
+++ b/Product Description/Klassen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DinoG\OneDrive\Desktop\Technisches Management 3. Semester\Software Engineering ILV\Git\Product Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B71460-5C3E-431E-B451-4D6174904069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91359429-52B7-45CA-A9F5-E9DADA52F9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EAE77123-B87F-48FC-8583-1A6EE0A6B883}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -274,13 +274,19 @@
   </si>
   <si>
     <t>printFleet()</t>
+  </si>
+  <si>
+    <t>Test-Elite</t>
+  </si>
+  <si>
+    <t>testNotDiagonalShip()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,12 +316,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -575,6 +575,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,18 +600,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -943,11 +943,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4191C2D1-8A23-4FA6-B2ED-476835485E0A}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R9" sqref="R9"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1003,24 +1003,24 @@
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="H3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="H3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="M3" s="18" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="M3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="20"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -1156,191 +1156,191 @@
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
       <c r="H9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
       <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="22"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
       <c r="H10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
       <c r="M10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="23" t="s">
+      <c r="N10" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="24"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="21"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="24"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
       <c r="M11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="23" t="s">
+      <c r="N11" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="24"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
       <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="24"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
       <c r="M12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="O12" s="23"/>
-      <c r="P12" s="24"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="21"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
       <c r="H13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="24"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
       <c r="M13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="24"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="21"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
       <c r="H14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
       <c r="M14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="24"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="21"/>
     </row>
     <row r="15" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
       <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="26"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="19"/>
       <c r="M15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="26"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="19"/>
     </row>
     <row r="17" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="20"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="20"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="24"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -1482,173 +1482,173 @@
       <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
       <c r="H24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="22"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
       <c r="M24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="22"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="24"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
       <c r="H25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="24"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
       <c r="M25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="24"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="21"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="C26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
       <c r="H26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="24"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
       <c r="M26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="24"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="21"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="C27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="24"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
       <c r="H27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="24"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21"/>
       <c r="M27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="24"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="21"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="C28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
       <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="24"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="21"/>
       <c r="M28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="24"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="21"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="C29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
       <c r="H29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="24"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
       <c r="M29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="24"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="21"/>
     </row>
     <row r="30" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="C30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
       <c r="H30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="26"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="19"/>
       <c r="M30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="26"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="19"/>
     </row>
     <row r="32" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
@@ -1711,88 +1711,272 @@
       <c r="C39" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="26"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="C40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="23" t="s">
+      <c r="D40" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="24"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="C41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="24"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="C42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="23"/>
-      <c r="F42" s="24"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="C43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="23"/>
-      <c r="F43" s="24"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="C44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="24"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="15"/>
       <c r="C45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="23"/>
-      <c r="F45" s="24"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="26"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="19"/>
+    </row>
+    <row r="49" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="24"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="14"/>
+      <c r="C52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="14"/>
+      <c r="C53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="14"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="15"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="4"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" s="25"/>
+      <c r="F56" s="26"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="14"/>
+      <c r="C57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="20"/>
+      <c r="F57" s="21"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="14"/>
+      <c r="C58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="21"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="14"/>
+      <c r="C59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="21"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="14"/>
+      <c r="C60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="21"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="14"/>
+      <c r="C61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="21"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="15"/>
+      <c r="C62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="21"/>
+    </row>
+    <row r="63" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C63" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="19"/>
+    </row>
+    <row r="64" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C64"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="66">
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D45:F45"/>
     <mergeCell ref="N30:P30"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="N10:P10"/>
@@ -1809,47 +1993,6 @@
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Testcases weiter geschrieben, Mario
</commit_message>
<xml_diff>
--- a/Product Description/Klassen.xlsx
+++ b/Product Description/Klassen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DinoG\OneDrive\Desktop\Technisches Management 3. Semester\Software Engineering ILV\Git\Product Description\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\IdeaProjects\TM22_SoftwareEngineering_Gruppe2\Product Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91359429-52B7-45CA-A9F5-E9DADA52F9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB32D88-8BF5-468D-8B68-5BF7ADB380FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EAE77123-B87F-48FC-8583-1A6EE0A6B883}"/>
   </bookViews>
@@ -40,7 +40,13 @@
     <author>tc={FCDDE2B2-D921-4040-B134-94E9E6B087D0}</author>
     <author>tc={9287C3D1-697B-408A-BE6F-8850285BA640}</author>
     <author>tc={8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}</author>
+    <author>tc={8344BD63-C90A-41CD-ACD3-87383028AAB7}</author>
+    <author>tc={CB7C96CB-1AEC-4C2E-930A-95BD6A3464BB}</author>
     <author>tc={0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}</author>
+    <author>tc={F5B95A25-956E-4D4A-9753-F211AF8BC6CA}</author>
+    <author>tc={9A86FC85-5D3E-4ADF-A608-3210D067A4E2}</author>
+    <author>tc={C393A2BB-2C26-488F-9665-8076CA409FF2}</author>
+    <author>tc={F2D28608-79FD-47A5-BB50-717AC6C57B41}</author>
   </authors>
   <commentList>
     <comment ref="N10" authorId="0" shapeId="0" xr:uid="{94C0B99F-C29B-43A8-935C-3212A1A77F9C}">
@@ -75,7 +81,23 @@
     Bitte Funktion implementieren, damit wir die Fleet ausgeben können</t>
       </text>
     </comment>
-    <comment ref="D28" authorId="4" shapeId="0" xr:uid="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
+    <comment ref="N13" authorId="4" shapeId="0" xr:uid="{8344BD63-C90A-41CD-ACD3-87383028AAB7}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben</t>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="5" shapeId="0" xr:uid="{CB7C96CB-1AEC-4C2E-930A-95BD6A3464BB}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    aufgespalten in printOwnField() und printOpponentField()</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="6" shapeId="0" xr:uid="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -83,12 +105,46 @@
     prints how many ships are sunk and how many are hit</t>
       </text>
     </comment>
+    <comment ref="D64" authorId="7" shapeId="0" xr:uid="{F5B95A25-956E-4D4A-9753-F211AF8BC6CA}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben
+Antwort:
+    Ruft auf : testFleetComplete und printFleet</t>
+      </text>
+    </comment>
+    <comment ref="D65" authorId="8" shapeId="0" xr:uid="{9A86FC85-5D3E-4ADF-A608-3210D067A4E2}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    ruft auf: checkIfSunk für TC-36.060</t>
+      </text>
+    </comment>
+    <comment ref="D66" authorId="9" shapeId="0" xr:uid="{C393A2BB-2C26-488F-9665-8076CA409FF2}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    gibt für TC-39.010 die größe des Feldes zurück</t>
+      </text>
+    </comment>
+    <comment ref="D67" authorId="10" shapeId="0" xr:uid="{F2D28608-79FD-47A5-BB50-717AC6C57B41}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    ruft auf: createField()</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -280,13 +336,34 @@
   </si>
   <si>
     <t>testNotDiagonalShip()</t>
+  </si>
+  <si>
+    <t>testFleetComplete()</t>
+  </si>
+  <si>
+    <t>printTestFleetComplete()</t>
+  </si>
+  <si>
+    <t>printSizeOfField(Field)</t>
+  </si>
+  <si>
+    <t>printCheckIfSunk(Ship)</t>
+  </si>
+  <si>
+    <t>printOwnField()</t>
+  </si>
+  <si>
+    <t>printOpponentField()</t>
+  </si>
+  <si>
+    <t>printTestField()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +393,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -556,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -575,16 +672,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -602,6 +702,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -622,6 +729,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Dino Ganic" id="{3BCCA9EA-61F7-4AAE-BD31-9F6FE5D618B8}" userId="4ed6363e1e8f2d27" providerId="Windows Live"/>
+  <person displayName="mario dangl" id="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" userId="7738e62b61fea53d" providerId="Windows Live"/>
   <person displayName="adri würfl" id="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" userId="c6b28034b5dd424b" providerId="Windows Live"/>
 </personList>
 </file>
@@ -935,19 +1043,40 @@
   <threadedComment ref="N12" dT="2021-09-25T15:35:38.57" personId="{3BCCA9EA-61F7-4AAE-BD31-9F6FE5D618B8}" id="{8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}">
     <text>Bitte Funktion implementieren, damit wir die Fleet ausgeben können</text>
   </threadedComment>
+  <threadedComment ref="N13" dT="2021-09-25T16:04:53.38" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{8344BD63-C90A-41CD-ACD3-87383028AAB7}">
+    <text>überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben</text>
+  </threadedComment>
+  <threadedComment ref="D27" dT="2021-09-25T16:36:37.64" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{CB7C96CB-1AEC-4C2E-930A-95BD6A3464BB}">
+    <text>aufgespalten in printOwnField() und printOpponentField()</text>
+  </threadedComment>
   <threadedComment ref="D28" dT="2021-09-25T10:33:50.75" personId="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" id="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
     <text>prints how many ships are sunk and how many are hit</text>
+  </threadedComment>
+  <threadedComment ref="D64" dT="2021-09-25T16:04:53.38" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{F5B95A25-956E-4D4A-9753-F211AF8BC6CA}">
+    <text>überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben</text>
+  </threadedComment>
+  <threadedComment ref="D64" dT="2021-09-25T16:08:16.61" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{8C06CD32-D7F2-4140-87A5-F6CF0057EEB4}" parentId="{F5B95A25-956E-4D4A-9753-F211AF8BC6CA}">
+    <text>Ruft auf : testFleetComplete und printFleet</text>
+  </threadedComment>
+  <threadedComment ref="D65" dT="2021-09-25T16:16:59.62" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{9A86FC85-5D3E-4ADF-A608-3210D067A4E2}">
+    <text>ruft auf: checkIfSunk für TC-36.060</text>
+  </threadedComment>
+  <threadedComment ref="D66" dT="2021-09-25T16:25:15.90" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{C393A2BB-2C26-488F-9665-8076CA409FF2}">
+    <text>gibt für TC-39.010 die größe des Feldes zurück</text>
+  </threadedComment>
+  <threadedComment ref="D67" dT="2021-09-25T16:40:39.87" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{F2D28608-79FD-47A5-BB50-717AC6C57B41}">
+    <text>ruft auf: createField()</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4191C2D1-8A23-4FA6-B2ED-476835485E0A}">
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58:F58"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1003,24 +1132,24 @@
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="H3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
-      <c r="M3" s="22" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="25"/>
+      <c r="M3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -1156,191 +1285,193 @@
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
       <c r="H9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
       <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="25" t="s">
+      <c r="N9" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="27"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
       <c r="H10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
       <c r="M10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
       <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
       <c r="M11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
       <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
       <c r="M12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="O12" s="20"/>
-      <c r="P12" s="21"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="20"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
       <c r="H13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
       <c r="M13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
+      <c r="N13" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13" s="19"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
       <c r="H14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="21"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
       <c r="M14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="20"/>
     </row>
     <row r="15" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
       <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
       <c r="M15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="19"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="22"/>
     </row>
     <row r="17" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="25"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="22" t="s">
+      <c r="M18" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="25"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -1482,460 +1613,670 @@
       <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
       <c r="H24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="27"/>
       <c r="M24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="27"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
       <c r="H25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="20"/>
       <c r="M25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="21"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="20"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="C26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
       <c r="H26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
       <c r="M26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="21"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="20"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="C27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
       <c r="H27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="21"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="20"/>
       <c r="M27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="21"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="20"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="C28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
       <c r="H28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="21"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="20"/>
       <c r="M28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="21"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="20"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="C29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
       <c r="H29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="20"/>
       <c r="M29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="21"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="30" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
-      <c r="C30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="C30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
       <c r="H30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="22"/>
       <c r="M30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="19"/>
-    </row>
-    <row r="32" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16" t="s">
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
+    </row>
+    <row r="31" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="C31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+    </row>
+    <row r="38" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C39" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="24"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="C35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="C36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="26"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="14"/>
-      <c r="C40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="C41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="C42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="14"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="15"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="26"/>
+      <c r="F45" s="27"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="14"/>
+      <c r="C46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="19"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="14"/>
+      <c r="C47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" s="19"/>
+      <c r="F47" s="20"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48" s="14"/>
+      <c r="C48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
-      <c r="C43" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D43" s="20" t="s">
+      <c r="E48" s="19"/>
+      <c r="F48" s="20"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="14"/>
+      <c r="C49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
-      <c r="C44" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44" s="20" t="s">
+      <c r="E49" s="19"/>
+      <c r="F49" s="20"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="14"/>
+      <c r="C50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="15"/>
-      <c r="C45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="20" t="s">
+      <c r="E50" s="19"/>
+      <c r="F50" s="20"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="15"/>
+      <c r="C51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C46" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
-    </row>
-    <row r="49" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="16" t="s">
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
+    </row>
+    <row r="52" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C52" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="55" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C56" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="24"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="17" t="s">
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="25"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="14"/>
-      <c r="C52" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
-      <c r="C53" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="14"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="5"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="15"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="4"/>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E56" s="25"/>
-      <c r="F56" s="26"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
-      <c r="C57" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E57" s="20"/>
-      <c r="F57" s="21"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="14"/>
       <c r="C58" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="21"/>
+        <v>4</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="14"/>
       <c r="C59" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="21"/>
+        <v>4</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="14"/>
-      <c r="C60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="21"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
-      <c r="C61" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="21"/>
+      <c r="A61" s="15"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="4"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="15"/>
-      <c r="C62" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="21"/>
-    </row>
-    <row r="63" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C63" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="19"/>
-    </row>
-    <row r="64" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C64"/>
+      <c r="A62" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" s="26"/>
+      <c r="F62" s="27"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="14"/>
+      <c r="C63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="19"/>
+      <c r="F63" s="20"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="14"/>
+      <c r="C64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E64" s="19"/>
+      <c r="F64" s="20"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="14"/>
+      <c r="C65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="26"/>
+      <c r="F65" s="27"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="14"/>
+      <c r="C66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E66" s="19"/>
+      <c r="F66" s="20"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="14"/>
+      <c r="C67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="19"/>
+      <c r="F67" s="20"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="15"/>
+      <c r="C68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="20"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="20"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="20"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="20"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="20"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="20"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="20"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="20"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="20"/>
+    </row>
+    <row r="77" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C77" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="75">
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="C56:F56"/>
     <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="D56:F56"/>
     <mergeCell ref="M3:P3"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N12:P12"/>
@@ -1950,49 +2291,13 @@
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D67:F67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implemented english outputs in whole programm for MVP
</commit_message>
<xml_diff>
--- a/Product Description/Klassen.xlsx
+++ b/Product Description/Klassen.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\IdeaProjects\TM22_SoftwareEngineering_Gruppe2\Product Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2644037C-43C6-496D-9896-DB1522D79A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8911D14-10A8-4977-9317-FCEA0ABA6DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{EAE77123-B87F-48FC-8583-1A6EE0A6B883}"/>
   </bookViews>
   <sheets>
     <sheet name="Klassen" sheetId="1" r:id="rId1"/>
+    <sheet name="game.java" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,16 @@
     <author>tc={94C0B99F-C29B-43A8-935C-3212A1A77F9C}</author>
     <author>tc={FCDDE2B2-D921-4040-B134-94E9E6B087D0}</author>
     <author>tc={9287C3D1-697B-408A-BE6F-8850285BA640}</author>
+    <author>tc={8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}</author>
+    <author>tc={8344BD63-C90A-41CD-ACD3-87383028AAB7}</author>
+    <author>tc={CB7C96CB-1AEC-4C2E-930A-95BD6A3464BB}</author>
     <author>tc={0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}</author>
+    <author>tc={12E0AA13-453A-40EE-AD6C-AE1B91326AA1}</author>
+    <author>tc={FF03A74C-8229-4277-88B5-1696134386C5}</author>
+    <author>tc={F5B95A25-956E-4D4A-9753-F211AF8BC6CA}</author>
+    <author>tc={9A86FC85-5D3E-4ADF-A608-3210D067A4E2}</author>
+    <author>tc={C393A2BB-2C26-488F-9665-8076CA409FF2}</author>
+    <author>tc={F2D28608-79FD-47A5-BB50-717AC6C57B41}</author>
   </authors>
   <commentList>
     <comment ref="N10" authorId="0" shapeId="0" xr:uid="{94C0B99F-C29B-43A8-935C-3212A1A77F9C}">
@@ -66,7 +76,31 @@
     sets all ships belonging to this fleet onto the field of the owner</t>
       </text>
     </comment>
-    <comment ref="D28" authorId="3" shapeId="0" xr:uid="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
+    <comment ref="N12" authorId="3" shapeId="0" xr:uid="{8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Bitte Funktion implementieren, damit wir die Fleet ausgeben können</t>
+      </text>
+    </comment>
+    <comment ref="N13" authorId="4" shapeId="0" xr:uid="{8344BD63-C90A-41CD-ACD3-87383028AAB7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben</t>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="5" shapeId="0" xr:uid="{CB7C96CB-1AEC-4C2E-930A-95BD6A3464BB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    aufgespalten in printOwnField() und printOpponentField()</t>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="6" shapeId="0" xr:uid="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,12 +108,63 @@
     prints how many ships are sunk and how many are hit</t>
       </text>
     </comment>
+    <comment ref="I37" authorId="7" shapeId="0" xr:uid="{12E0AA13-453A-40EE-AD6C-AE1B91326AA1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Gibt die anzahl an durchgeführten Spiezügen an</t>
+      </text>
+    </comment>
+    <comment ref="I38" authorId="8" shapeId="0" xr:uid="{FF03A74C-8229-4277-88B5-1696134386C5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    gibt an welcher spieler an der Reihe ist -&gt; wenn true = spieler 1, wenn false spieler 2;
+Wird nach Beendigung eines Spielzuges umgedreht</t>
+      </text>
+    </comment>
+    <comment ref="D61" authorId="9" shapeId="0" xr:uid="{F5B95A25-956E-4D4A-9753-F211AF8BC6CA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben
+Reply:
+    Ruft auf : testFleetComplete und printFleet</t>
+      </text>
+    </comment>
+    <comment ref="D62" authorId="10" shapeId="0" xr:uid="{9A86FC85-5D3E-4ADF-A608-3210D067A4E2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ruft auf: checkIfSunk für TC-36.060</t>
+      </text>
+    </comment>
+    <comment ref="D63" authorId="11" shapeId="0" xr:uid="{C393A2BB-2C26-488F-9665-8076CA409FF2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    gibt für TC-39.010 die größe des Feldes zurück</t>
+      </text>
+    </comment>
+    <comment ref="D64" authorId="12" shapeId="0" xr:uid="{F2D28608-79FD-47A5-BB50-717AC6C57B41}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ruft auf: createField()</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -165,9 +250,6 @@
     <t>positionY</t>
   </si>
   <si>
-    <t>shotAt</t>
-  </si>
-  <si>
     <t>target</t>
   </si>
   <si>
@@ -262,13 +344,70 @@
   </si>
   <si>
     <t>createPlayer(name)</t>
+  </si>
+  <si>
+    <t>printFleet()</t>
+  </si>
+  <si>
+    <t>testNotDiagonalShip()</t>
+  </si>
+  <si>
+    <t>testFleetComplete()</t>
+  </si>
+  <si>
+    <t>printTestFleetComplete()</t>
+  </si>
+  <si>
+    <t>printSizeOfField(Field)</t>
+  </si>
+  <si>
+    <t>printCheckIfSunk(Ship)</t>
+  </si>
+  <si>
+    <t>printOwnField()</t>
+  </si>
+  <si>
+    <t>printOpponentField()</t>
+  </si>
+  <si>
+    <t>printTestField()</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>player1</t>
+  </si>
+  <si>
+    <t>default:true</t>
+  </si>
+  <si>
+    <t>default:0</t>
+  </si>
+  <si>
+    <t>Main function</t>
+  </si>
+  <si>
+    <t>Setupgame</t>
+  </si>
+  <si>
+    <t>Setup_Game</t>
+  </si>
+  <si>
+    <t>opponentField</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +433,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -544,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -563,16 +710,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -588,6 +739,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -609,6 +766,8 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Dino Ganic" id="{3BCCA9EA-61F7-4AAE-BD31-9F6FE5D618B8}" userId="4ed6363e1e8f2d27" providerId="Windows Live"/>
+  <person displayName="mario dangl" id="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" userId="7738e62b61fea53d" providerId="Windows Live"/>
   <person displayName="adri würfl" id="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" userId="c6b28034b5dd424b" providerId="Windows Live"/>
 </personList>
 </file>
@@ -919,28 +1078,59 @@
   <threadedComment ref="N11" dT="2021-09-25T13:55:58.73" personId="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" id="{9287C3D1-697B-408A-BE6F-8850285BA640}">
     <text>sets all ships belonging to this fleet onto the field of the owner</text>
   </threadedComment>
+  <threadedComment ref="N12" dT="2021-09-25T15:35:38.57" personId="{3BCCA9EA-61F7-4AAE-BD31-9F6FE5D618B8}" id="{8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}">
+    <text>Bitte Funktion implementieren, damit wir die Fleet ausgeben können</text>
+  </threadedComment>
+  <threadedComment ref="N13" dT="2021-09-25T16:04:53.38" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{8344BD63-C90A-41CD-ACD3-87383028AAB7}">
+    <text>überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben</text>
+  </threadedComment>
+  <threadedComment ref="D27" dT="2021-09-25T16:36:37.64" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{CB7C96CB-1AEC-4C2E-930A-95BD6A3464BB}">
+    <text>aufgespalten in printOwnField() und printOpponentField()</text>
+  </threadedComment>
   <threadedComment ref="D28" dT="2021-09-25T10:33:50.75" personId="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" id="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
     <text>prints how many ships are sunk and how many are hit</text>
+  </threadedComment>
+  <threadedComment ref="I37" dT="2021-09-27T14:34:39.96" personId="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" id="{12E0AA13-453A-40EE-AD6C-AE1B91326AA1}">
+    <text>Gibt die anzahl an durchgeführten Spiezügen an</text>
+  </threadedComment>
+  <threadedComment ref="I38" dT="2021-09-27T14:34:23.27" personId="{6B23838A-6FAD-4E26-82A7-3F5739AFD6B0}" id="{FF03A74C-8229-4277-88B5-1696134386C5}">
+    <text>gibt an welcher spieler an der Reihe ist -&gt; wenn true = spieler 1, wenn false spieler 2;
+Wird nach Beendigung eines Spielzuges umgedreht</text>
+  </threadedComment>
+  <threadedComment ref="D61" dT="2021-09-25T16:04:53.38" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{F5B95A25-956E-4D4A-9753-F211AF8BC6CA}">
+    <text>überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben</text>
+  </threadedComment>
+  <threadedComment ref="D61" dT="2021-09-25T16:08:16.61" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{8C06CD32-D7F2-4140-87A5-F6CF0057EEB4}" parentId="{F5B95A25-956E-4D4A-9753-F211AF8BC6CA}">
+    <text>Ruft auf : testFleetComplete und printFleet</text>
+  </threadedComment>
+  <threadedComment ref="D62" dT="2021-09-25T16:16:59.62" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{9A86FC85-5D3E-4ADF-A608-3210D067A4E2}">
+    <text>ruft auf: checkIfSunk für TC-36.060</text>
+  </threadedComment>
+  <threadedComment ref="D63" dT="2021-09-25T16:25:15.90" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{C393A2BB-2C26-488F-9665-8076CA409FF2}">
+    <text>gibt für TC-39.010 die größe des Feldes zurück</text>
+  </threadedComment>
+  <threadedComment ref="D64" dT="2021-09-25T16:40:39.87" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{F2D28608-79FD-47A5-BB50-717AC6C57B41}">
+    <text>ruft auf: createField()</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4191C2D1-8A23-4FA6-B2ED-476835485E0A}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="1.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="1.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.53125" bestFit="1" customWidth="1"/>
@@ -959,7 +1149,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="11" t="s">
@@ -969,7 +1159,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M1" s="10"/>
       <c r="N1" s="11" t="s">
@@ -979,7 +1169,7 @@
         <v>6</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -987,24 +1177,24 @@
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="H3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
-      <c r="M3" s="22" t="s">
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
+      <c r="M3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A4" s="17" t="s">
@@ -1034,7 +1224,7 @@
         <v>4</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>18</v>
@@ -1063,7 +1253,7 @@
         <v>11</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>4</v>
@@ -1084,7 +1274,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>4</v>
@@ -1140,27 +1330,27 @@
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
       <c r="H9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
       <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="26"/>
+      <c r="N9" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="27"/>
+      <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A10" s="14"/>
@@ -1176,7 +1366,7 @@
         <v>12</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="21"/>
@@ -1184,7 +1374,7 @@
         <v>12</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O10" s="20"/>
       <c r="P10" s="21"/>
@@ -1209,7 +1399,7 @@
         <v>12</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O11" s="20"/>
       <c r="P11" s="21"/>
@@ -1231,7 +1421,9 @@
       <c r="M12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="20"/>
+      <c r="N12" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="O12" s="20"/>
       <c r="P12" s="21"/>
     </row>
@@ -1252,7 +1444,9 @@
       <c r="M13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="20"/>
+      <c r="N13" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="O13" s="20"/>
       <c r="P13" s="21"/>
     </row>
@@ -1282,47 +1476,47 @@
       <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23"/>
       <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
       <c r="M15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="19"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
     </row>
     <row r="17" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="18" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="22" t="s">
+      <c r="M18" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="24"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A19" s="17" t="s">
@@ -1332,7 +1526,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>18</v>
@@ -1342,7 +1536,7 @@
         <v>4</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>21</v>
@@ -1371,13 +1565,13 @@
         <v>7</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>18</v>
@@ -1400,13 +1594,13 @@
         <v>4</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>4</v>
@@ -1417,15 +1611,9 @@
       <c r="M21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A22" s="14"/>
@@ -1464,25 +1652,25 @@
       <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
+      <c r="D24" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="28"/>
       <c r="H24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
+      <c r="I24" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="28"/>
       <c r="M24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="26"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="28"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A25" s="14"/>
@@ -1490,7 +1678,7 @@
         <v>12</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="21"/>
@@ -1513,7 +1701,7 @@
         <v>12</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="21"/>
@@ -1535,11 +1723,11 @@
       <c r="C27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
+      <c r="D27" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="29"/>
+      <c r="F27" s="30"/>
       <c r="H27" s="3" t="s">
         <v>12</v>
       </c>
@@ -1559,7 +1747,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="21"/>
@@ -1582,7 +1770,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="21"/>
@@ -1601,180 +1789,547 @@
     </row>
     <row r="30" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="15"/>
-      <c r="C30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
+      <c r="C30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
       <c r="H30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="23"/>
       <c r="M30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="19"/>
-    </row>
-    <row r="32" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="33" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="16" t="s">
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="23"/>
+    </row>
+    <row r="31" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="4"/>
+      <c r="C31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="22"/>
+      <c r="F31" s="23"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A32" s="4"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A33" s="4"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+    </row>
+    <row r="35" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="36" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C36" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="24"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A34" s="17" t="s">
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="26"/>
+      <c r="H36" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="26"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A35" s="14"/>
-      <c r="C35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="F37" s="5"/>
+      <c r="H37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A38" s="14"/>
+      <c r="C38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A36" s="14"/>
-      <c r="C36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A37" s="14"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A38" s="15"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
       <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A39" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="26"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="H38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A39" s="14"/>
+      <c r="C39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="H39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A40" s="14"/>
       <c r="C40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A41" s="14"/>
-      <c r="C41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A42" s="14"/>
-      <c r="C42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+        <v>4</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A41" s="15"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="F41" s="5"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A42" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
+      <c r="H42" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="28"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A43" s="14"/>
       <c r="C43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="H43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="21"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A44" s="14"/>
       <c r="C44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A45" s="15"/>
+      <c r="H44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="21"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A45" s="14"/>
       <c r="C45" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C46" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19"/>
+      <c r="H45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="21"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A46" s="14"/>
+      <c r="C46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
+      <c r="H46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="21"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A47" s="14"/>
+      <c r="C47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
+      <c r="H47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="21"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A48" s="15"/>
+      <c r="C48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21"/>
+      <c r="H48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="21"/>
+    </row>
+    <row r="49" spans="1:11" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C49" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="23"/>
+      <c r="H49" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="23"/>
+    </row>
+    <row r="52" spans="1:11" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="53" spans="1:11" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="26"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A54" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A55" s="14"/>
+      <c r="C55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A56" s="14"/>
+      <c r="C56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A57" s="14"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A58" s="15"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="4"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A59" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" s="27"/>
+      <c r="F59" s="28"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A60" s="14"/>
+      <c r="C60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" s="20"/>
+      <c r="F60" s="21"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A61" s="14"/>
+      <c r="C61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" s="20"/>
+      <c r="F61" s="21"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A62" s="14"/>
+      <c r="C62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="27"/>
+      <c r="F62" s="28"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A63" s="14"/>
+      <c r="C63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" s="20"/>
+      <c r="F63" s="21"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A64" s="14"/>
+      <c r="C64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="20"/>
+      <c r="F64" s="21"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A65" s="15"/>
+      <c r="C65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="21"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="21"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="21"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="21"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="21"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="21"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="21"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="21"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="21"/>
+    </row>
+    <row r="74" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C74" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
+  <mergeCells count="84">
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="D59:F59"/>
     <mergeCell ref="M3:P3"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N12:P12"/>
@@ -1789,6 +2344,7 @@
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="I9:K9"/>
+    <mergeCell ref="D48:F48"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="D13:F13"/>
@@ -1802,24 +2358,18 @@
     <mergeCell ref="N24:P24"/>
     <mergeCell ref="N26:P26"/>
     <mergeCell ref="N27:P27"/>
-    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="I42:K42"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="I28:K28"/>
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="I30:K30"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D45:F45"/>
     <mergeCell ref="N30:P30"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D43:F43"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="I25:K25"/>
     <mergeCell ref="N25:P25"/>
@@ -1832,9 +2382,164 @@
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FAE8B0-E1EB-459D-B352-9E383FBDE9C3}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="1.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="2:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implemented in FlowGameOver query "Play Again" or "Quit Game";  implemented in Main loop do while (gameover false), Mario
</commit_message>
<xml_diff>
--- a/Product Description/Klassen.xlsx
+++ b/Product Description/Klassen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\IdeaProjects\TM22_SoftwareEngineering_Gruppe2\Product Description\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\IdeaProjects\TM22_SoftwareEngineering_Gruppe2\Product Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8911D14-10A8-4977-9317-FCEA0ABA6DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7553084-A43E-4F04-A6B8-BBC0C8153619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{EAE77123-B87F-48FC-8583-1A6EE0A6B883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EAE77123-B87F-48FC-8583-1A6EE0A6B883}"/>
   </bookViews>
   <sheets>
     <sheet name="Klassen" sheetId="1" r:id="rId1"/>
@@ -54,108 +54,108 @@
   <commentList>
     <comment ref="N10" authorId="0" shapeId="0" xr:uid="{94C0B99F-C29B-43A8-935C-3212A1A77F9C}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     creates ships randomly &amp; then sets it onto the field</t>
       </text>
     </comment>
     <comment ref="D11" authorId="1" shapeId="0" xr:uid="{FCDDE2B2-D921-4040-B134-94E9E6B087D0}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     Hier muss überprüft werden ob ship mit flotte kompatibel ist (ob nicht andere schiffe im Weg stehen ^^)</t>
       </text>
     </comment>
     <comment ref="N11" authorId="2" shapeId="0" xr:uid="{9287C3D1-697B-408A-BE6F-8850285BA640}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     sets all ships belonging to this fleet onto the field of the owner</t>
       </text>
     </comment>
     <comment ref="N12" authorId="3" shapeId="0" xr:uid="{8B24ACCE-611F-40D2-A745-5DA1D7CFE2E6}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     Bitte Funktion implementieren, damit wir die Fleet ausgeben können</t>
       </text>
     </comment>
     <comment ref="N13" authorId="4" shapeId="0" xr:uid="{8344BD63-C90A-41CD-ACD3-87383028AAB7}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben</t>
       </text>
     </comment>
     <comment ref="D27" authorId="5" shapeId="0" xr:uid="{CB7C96CB-1AEC-4C2E-930A-95BD6A3464BB}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     aufgespalten in printOwnField() und printOpponentField()</t>
       </text>
     </comment>
     <comment ref="D28" authorId="6" shapeId="0" xr:uid="{0A20BC7B-BCF6-4657-A941-3DE5A11F61D8}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     prints how many ships are sunk and how many are hit</t>
       </text>
     </comment>
     <comment ref="I37" authorId="7" shapeId="0" xr:uid="{12E0AA13-453A-40EE-AD6C-AE1B91326AA1}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     Gibt die anzahl an durchgeführten Spiezügen an</t>
       </text>
     </comment>
     <comment ref="I38" authorId="8" shapeId="0" xr:uid="{FF03A74C-8229-4277-88B5-1696134386C5}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     gibt an welcher spieler an der Reihe ist -&gt; wenn true = spieler 1, wenn false spieler 2;
 Wird nach Beendigung eines Spielzuges umgedreht</t>
       </text>
     </comment>
     <comment ref="D61" authorId="9" shapeId="0" xr:uid="{F5B95A25-956E-4D4A-9753-F211AF8BC6CA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     überprüfung ob alle 10 Schiffe vorhanden, und die richtigen Größen (siehe Anf.) haben
-Reply:
+Antwort:
     Ruft auf : testFleetComplete und printFleet</t>
       </text>
     </comment>
     <comment ref="D62" authorId="10" shapeId="0" xr:uid="{9A86FC85-5D3E-4ADF-A608-3210D067A4E2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     ruft auf: checkIfSunk für TC-36.060</t>
       </text>
     </comment>
     <comment ref="D63" authorId="11" shapeId="0" xr:uid="{C393A2BB-2C26-488F-9665-8076CA409FF2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     gibt für TC-39.010 die größe des Feldes zurück</t>
       </text>
     </comment>
     <comment ref="D64" authorId="12" shapeId="0" xr:uid="{F2D28608-79FD-47A5-BB50-717AC6C57B41}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     ruft auf: createField()</t>
       </text>
     </comment>
@@ -163,8 +163,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1F53BDD1-D313-4A2D-AC21-2765BFA22B25}</author>
+  </authors>
+  <commentList>
+    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{1F53BDD1-D313-4A2D-AC21-2765BFA22B25}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    redirect zu entscheidung zu funktionen "weiterspielen" oder "beenden" oder "highscore" ...</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -401,6 +419,21 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>+ next steps</t>
+  </si>
+  <si>
+    <t>checkIfHit()</t>
+  </si>
+  <si>
+    <t>checkIfShotHit()</t>
+  </si>
+  <si>
+    <t>checkWhichShipIsHere(Coordinate)</t>
+  </si>
+  <si>
+    <t>checkWhichShipWasShot(Shot)</t>
   </si>
 </sst>
 </file>
@@ -449,7 +482,7 @@
     <font>
       <sz val="9"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
+      <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -691,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -726,6 +759,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -735,21 +774,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,7 +807,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1115,32 +1149,40 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I22" dT="2021-09-27T17:36:29.85" personId="{A338ACA1-BBDB-4216-85CD-7914FF1BE1E5}" id="{1F53BDD1-D313-4A2D-AC21-2765BFA22B25}">
+    <text>redirect zu entscheidung zu funktionen "weiterspielen" oder "beenden" oder "highscore" ...</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4191C2D1-8A23-4FA6-B2ED-476835485E0A}">
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28:K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
-    <col min="3" max="3" width="1.46484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.77734375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C1" s="10"/>
       <c r="D1" s="11" t="s">
         <v>0</v>
@@ -1172,31 +1214,31 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="H3" s="24" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="H3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
-      <c r="M3" s="24" t="s">
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="28"/>
+      <c r="M3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="26"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="28"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
@@ -1231,7 +1273,7 @@
       </c>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -1262,7 +1304,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
@@ -1293,7 +1335,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
@@ -1308,7 +1350,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
@@ -1323,36 +1365,36 @@
       <c r="O8" s="4"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
       <c r="H9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
       <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="27" t="s">
+      <c r="N9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="28"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="O9" s="24"/>
+      <c r="P9" s="25"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="C10" s="3" t="s">
         <v>12</v>
@@ -1379,7 +1421,7 @@
       <c r="O10" s="20"/>
       <c r="P10" s="21"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="C11" s="3" t="s">
         <v>12</v>
@@ -1404,12 +1446,14 @@
       <c r="O11" s="20"/>
       <c r="P11" s="21"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="20"/>
+      <c r="D12" s="20" t="s">
+        <v>80</v>
+      </c>
       <c r="E12" s="20"/>
       <c r="F12" s="21"/>
       <c r="H12" s="3" t="s">
@@ -1427,7 +1471,7 @@
       <c r="O12" s="20"/>
       <c r="P12" s="21"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="C13" s="3" t="s">
         <v>12</v>
@@ -1450,7 +1494,7 @@
       <c r="O13" s="20"/>
       <c r="P13" s="21"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="C14" s="3" t="s">
         <v>12</v>
@@ -1471,7 +1515,7 @@
       <c r="O14" s="20"/>
       <c r="P14" s="21"/>
     </row>
-    <row r="15" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="C15" s="6" t="s">
         <v>12</v>
@@ -1492,33 +1536,33 @@
       <c r="O15" s="22"/>
       <c r="P15" s="23"/>
     </row>
-    <row r="17" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="18" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="26"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="28"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="24" t="s">
+      <c r="M18" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="26"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="28"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>1</v>
       </c>
@@ -1553,7 +1597,7 @@
       </c>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="C20" s="3" t="s">
         <v>4</v>
@@ -1588,7 +1632,7 @@
       </c>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="C21" s="3" t="s">
         <v>4</v>
@@ -1615,7 +1659,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
@@ -1630,7 +1674,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
@@ -1645,34 +1689,34 @@
       <c r="O23" s="4"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="25"/>
       <c r="H24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="27" t="s">
+      <c r="I24" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="25"/>
       <c r="M24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="28"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="25"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>12</v>
@@ -1685,7 +1729,9 @@
       <c r="H25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="20"/>
+      <c r="I25" s="20" t="s">
+        <v>81</v>
+      </c>
       <c r="J25" s="20"/>
       <c r="K25" s="21"/>
       <c r="M25" s="3" t="s">
@@ -1695,7 +1741,7 @@
       <c r="O25" s="20"/>
       <c r="P25" s="21"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="C26" s="3" t="s">
         <v>12</v>
@@ -1718,7 +1764,7 @@
       <c r="O26" s="20"/>
       <c r="P26" s="21"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="C27" s="3" t="s">
         <v>12</v>
@@ -1741,7 +1787,7 @@
       <c r="O27" s="20"/>
       <c r="P27" s="21"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="C28" s="3" t="s">
         <v>12</v>
@@ -1764,7 +1810,7 @@
       <c r="O28" s="20"/>
       <c r="P28" s="21"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="C29" s="3" t="s">
         <v>12</v>
@@ -1787,7 +1833,7 @@
       <c r="O29" s="20"/>
       <c r="P29" s="21"/>
     </row>
-    <row r="30" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="C30" s="3" t="s">
         <v>12</v>
@@ -1810,16 +1856,16 @@
       <c r="O30" s="22"/>
       <c r="P30" s="23"/>
     </row>
-    <row r="31" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
-      <c r="C31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="22" t="s">
+      <c r="C31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="23"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
       <c r="H31" s="19"/>
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
@@ -1829,12 +1875,16 @@
       <c r="O31" s="18"/>
       <c r="P31" s="18"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="C32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
       <c r="H32" s="19"/>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
@@ -1844,12 +1894,16 @@
       <c r="O32" s="18"/>
       <c r="P32" s="18"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
+      <c r="C33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="23"/>
       <c r="H33" s="19"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
@@ -1859,25 +1913,25 @@
       <c r="O33" s="18"/>
       <c r="P33" s="18"/>
     </row>
-    <row r="35" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="36" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
-      <c r="H36" s="24" t="s">
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="28"/>
+      <c r="H36" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="26"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="28"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>1</v>
       </c>
@@ -1904,7 +1958,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="C38" s="3" t="s">
         <v>4</v>
@@ -1929,7 +1983,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="C39" s="3" t="s">
         <v>4</v>
@@ -1948,7 +2002,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="C40" s="3" t="s">
         <v>4</v>
@@ -1965,7 +2019,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
@@ -1974,26 +2028,26 @@
       <c r="I41" s="4"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="27"/>
-      <c r="F42" s="28"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="25"/>
       <c r="H42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="28"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="25"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="C43" s="3" t="s">
         <v>12</v>
@@ -2010,7 +2064,7 @@
       <c r="J43" s="20"/>
       <c r="K43" s="21"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="C44" s="3" t="s">
         <v>12</v>
@@ -2027,7 +2081,7 @@
       <c r="J44" s="20"/>
       <c r="K44" s="21"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="C45" s="3" t="s">
         <v>12</v>
@@ -2044,7 +2098,7 @@
       <c r="J45" s="20"/>
       <c r="K45" s="21"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
       <c r="C46" s="3" t="s">
         <v>12</v>
@@ -2061,7 +2115,7 @@
       <c r="J46" s="20"/>
       <c r="K46" s="21"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="14"/>
       <c r="C47" s="3" t="s">
         <v>12</v>
@@ -2078,7 +2132,7 @@
       <c r="J47" s="20"/>
       <c r="K47" s="21"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="15"/>
       <c r="C48" s="3" t="s">
         <v>12</v>
@@ -2095,7 +2149,7 @@
       <c r="J48" s="20"/>
       <c r="K48" s="21"/>
     </row>
-    <row r="49" spans="1:11" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C49" s="6" t="s">
         <v>12</v>
       </c>
@@ -2109,19 +2163,19 @@
       <c r="J49" s="22"/>
       <c r="K49" s="23"/>
     </row>
-    <row r="52" spans="1:11" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="53" spans="1:11" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="26"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="28"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>1</v>
       </c>
@@ -2132,7 +2186,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="14"/>
       <c r="C55" s="3" t="s">
         <v>4</v>
@@ -2141,7 +2195,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="5"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="14"/>
       <c r="C56" s="3" t="s">
         <v>4</v>
@@ -2150,33 +2204,33 @@
       <c r="E56" s="4"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="14"/>
       <c r="C57" s="3"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="15"/>
       <c r="C58" s="3"/>
       <c r="D58" s="4"/>
       <c r="F58" s="5"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D59" s="27" t="s">
+      <c r="D59" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="27"/>
-      <c r="F59" s="28"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="E59" s="24"/>
+      <c r="F59" s="25"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="14"/>
       <c r="C60" s="3" t="s">
         <v>12</v>
@@ -2187,7 +2241,7 @@
       <c r="E60" s="20"/>
       <c r="F60" s="21"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="14"/>
       <c r="C61" s="3" t="s">
         <v>12</v>
@@ -2198,18 +2252,18 @@
       <c r="E61" s="20"/>
       <c r="F61" s="21"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="14"/>
       <c r="C62" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D62" s="27" t="s">
+      <c r="D62" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="27"/>
-      <c r="F62" s="28"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="E62" s="24"/>
+      <c r="F62" s="25"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="14"/>
       <c r="C63" s="3" t="s">
         <v>12</v>
@@ -2220,7 +2274,7 @@
       <c r="E63" s="20"/>
       <c r="F63" s="21"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="14"/>
       <c r="C64" s="3" t="s">
         <v>12</v>
@@ -2231,7 +2285,7 @@
       <c r="E64" s="20"/>
       <c r="F64" s="21"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="15"/>
       <c r="C65" s="3" t="s">
         <v>12</v>
@@ -2240,7 +2294,7 @@
       <c r="E65" s="20"/>
       <c r="F65" s="21"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C66" s="3" t="s">
         <v>12</v>
       </c>
@@ -2248,7 +2302,7 @@
       <c r="E66" s="20"/>
       <c r="F66" s="21"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C67" s="3" t="s">
         <v>12</v>
       </c>
@@ -2256,7 +2310,7 @@
       <c r="E67" s="20"/>
       <c r="F67" s="21"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
         <v>12</v>
       </c>
@@ -2264,7 +2318,7 @@
       <c r="E68" s="20"/>
       <c r="F68" s="21"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C69" s="3" t="s">
         <v>12</v>
       </c>
@@ -2272,7 +2326,7 @@
       <c r="E69" s="20"/>
       <c r="F69" s="21"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C70" s="3" t="s">
         <v>12</v>
       </c>
@@ -2280,7 +2334,7 @@
       <c r="E70" s="20"/>
       <c r="F70" s="21"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C71" s="3" t="s">
         <v>12</v>
       </c>
@@ -2288,7 +2342,7 @@
       <c r="E71" s="20"/>
       <c r="F71" s="21"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C72" s="3" t="s">
         <v>12</v>
       </c>
@@ -2296,7 +2350,7 @@
       <c r="E72" s="20"/>
       <c r="F72" s="21"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C73" s="3" t="s">
         <v>12</v>
       </c>
@@ -2304,7 +2358,7 @@
       <c r="E73" s="20"/>
       <c r="F73" s="21"/>
     </row>
-    <row r="74" spans="1:6" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C74" s="6" t="s">
         <v>12</v>
       </c>
@@ -2313,21 +2367,63 @@
       <c r="F74" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
+  <mergeCells count="86">
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="I42:K42"/>
     <mergeCell ref="C53:F53"/>
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="M3:P3"/>
@@ -2344,60 +2440,20 @@
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="I9:K9"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2406,38 +2462,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FAE8B0-E1EB-459D-B352-9E383FBDE9C3}">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FAE8B0-E1EB-459D-B352-9E383FBDE9C3}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="1.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="24" t="s">
+    <row r="6" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2445,7 +2501,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2453,7 +2509,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -2461,27 +2517,27 @@
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2489,7 +2545,7 @@
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2497,7 +2553,7 @@
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
@@ -2505,7 +2561,7 @@
       <c r="D15" s="20"/>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
@@ -2513,7 +2569,7 @@
       <c r="D16" s="20"/>
       <c r="E16" s="21"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
@@ -2521,13 +2577,18 @@
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
     </row>
-    <row r="18" spans="2:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I22" s="31" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2541,5 +2602,6 @@
     <mergeCell ref="C16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>